<commit_message>
Update id and new template anssi framework
</commit_message>
<xml_diff>
--- a/tools/anssi/anssi-recommandations-configuration-systeme-gnu-linux.xlsx
+++ b/tools/anssi/anssi-recommandations-configuration-systeme-gnu-linux.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="368">
   <si>
     <t>library_urn</t>
   </si>
@@ -33,7 +33,7 @@
     <t>library_ref_id</t>
   </si>
   <si>
-    <t>ANSSI</t>
+    <t>ANSSI-REC-LINUX</t>
   </si>
   <si>
     <t>library_name</t>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>library_provider</t>
+  </si>
+  <si>
+    <t>ANSSI</t>
   </si>
   <si>
     <t>library_packager</t>
@@ -3574,7 +3577,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3582,10 +3585,10 @@
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3593,10 +3596,10 @@
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3604,7 +3607,7 @@
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s" s="3">
         <v>6</v>
@@ -3615,7 +3618,7 @@
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s" s="3">
         <v>8</v>
@@ -3626,10 +3629,10 @@
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3637,26 +3640,26 @@
     </row>
     <row r="14" ht="17" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -3688,22 +3691,22 @@
   <sheetData>
     <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="B1" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s" s="10">
-        <v>25</v>
-      </c>
       <c r="D1" t="s" s="11">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s" s="12">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="17" customHeight="1">
@@ -3713,10 +3716,10 @@
       </c>
       <c r="C2" s="14"/>
       <c r="D2" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s" s="12">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -3727,31 +3730,31 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" ht="272" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s" s="12">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s" s="12">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" ht="255" customHeight="1">
@@ -3761,31 +3764,31 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s" s="12">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" ht="255" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="13">
         <v>3</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s" s="12">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s" s="12">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" ht="238" customHeight="1">
@@ -3795,10 +3798,10 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s" s="12">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F7" s="15"/>
     </row>
@@ -3809,31 +3812,31 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s" s="12">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" s="15"/>
     </row>
     <row r="9" ht="238" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="13">
         <v>4</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s" s="12">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s" s="12">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" ht="17" customHeight="1">
@@ -3843,31 +3846,31 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s" s="12">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="13">
         <v>4</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s" s="12">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" ht="136" customHeight="1">
@@ -3877,10 +3880,10 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s" s="12">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" s="15"/>
     </row>
@@ -3891,31 +3894,31 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s" s="12">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F13" s="15"/>
     </row>
     <row r="14" ht="136" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="13">
         <v>3</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s" s="12">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s" s="12">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" ht="204" customHeight="1">
@@ -3925,31 +3928,31 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s" s="12">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="15"/>
     </row>
     <row r="16" ht="204" customHeight="1">
       <c r="A16" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="13">
         <v>3</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s" s="12">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s" s="12">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" ht="170" customHeight="1">
@@ -3959,51 +3962,51 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s" s="12">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="15"/>
     </row>
     <row r="18" ht="170" customHeight="1">
       <c r="A18" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="13">
         <v>4</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s" s="12">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s" s="12">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" ht="187" customHeight="1">
       <c r="A19" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="13">
         <v>4</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s" s="12">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s" s="12">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" ht="17" customHeight="1">
@@ -4013,51 +4016,51 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s" s="12">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" ht="353" customHeight="1">
       <c r="A21" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="13">
         <v>4</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s" s="12">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s" s="12">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" ht="187" customHeight="1">
       <c r="A22" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="13">
         <v>4</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s" s="12">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F22" t="s" s="12">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" ht="153" customHeight="1">
@@ -4067,31 +4070,31 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s" s="12">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F23" s="15"/>
     </row>
     <row r="24" ht="153" customHeight="1">
       <c r="A24" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="13">
         <v>4</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s" s="12">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F24" t="s" s="12">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" ht="17" customHeight="1">
@@ -4101,51 +4104,51 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s" s="12">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F25" s="15"/>
     </row>
     <row r="26" ht="871" customHeight="1">
       <c r="A26" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="13">
         <v>4</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E26" t="s" s="12">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s" s="12">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" ht="191.55" customHeight="1">
       <c r="A27" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="13">
         <v>4</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s" s="12">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s" s="12">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" ht="170" customHeight="1">
@@ -4155,31 +4158,31 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s" s="12">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F28" s="15"/>
     </row>
     <row r="29" ht="325" customHeight="1">
       <c r="A29" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="13">
         <v>4</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s" s="12">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F29" t="s" s="12">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" ht="153" customHeight="1">
@@ -4189,10 +4192,10 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E30" t="s" s="12">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F30" s="15"/>
     </row>
@@ -4203,191 +4206,191 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s" s="12">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="15"/>
     </row>
     <row r="32" ht="815" customHeight="1">
       <c r="A32" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B32" s="13">
         <v>4</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s" s="12">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s" s="12">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" ht="199" customHeight="1">
       <c r="A33" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="13">
         <v>4</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E33" t="s" s="12">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s" s="12">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" ht="367" customHeight="1">
       <c r="A34" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" s="13">
         <v>4</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E34" t="s" s="12">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F34" t="s" s="12">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" ht="311" customHeight="1">
       <c r="A35" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" s="13">
         <v>4</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E35" t="s" s="12">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s" s="12">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" ht="185" customHeight="1">
       <c r="A36" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="13">
         <v>4</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E36" t="s" s="12">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F36" t="s" s="12">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" ht="283" customHeight="1">
       <c r="A37" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="13">
         <v>4</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E37" t="s" s="12">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F37" t="s" s="12">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" ht="297" customHeight="1">
       <c r="A38" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="13">
         <v>4</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s" s="12">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s" s="12">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" ht="115" customHeight="1">
       <c r="A39" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="13">
         <v>4</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E39" t="s" s="12">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F39" t="s" s="12">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" ht="255" customHeight="1">
       <c r="A40" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B40" s="13">
         <v>4</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E40" t="s" s="12">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s" s="12">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" ht="221" customHeight="1">
@@ -4397,91 +4400,91 @@
       </c>
       <c r="C41" s="4"/>
       <c r="D41" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s" s="12">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F41" s="15"/>
     </row>
     <row r="42" ht="185" customHeight="1">
       <c r="A42" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B42" s="13">
         <v>4</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E42" t="s" s="12">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F42" t="s" s="12">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" ht="311" customHeight="1">
       <c r="A43" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B43" s="13">
         <v>4</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s" s="12">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F43" t="s" s="12">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" ht="213" customHeight="1">
       <c r="A44" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B44" s="13">
         <v>4</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E44" t="s" s="12">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F44" t="s" s="12">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" ht="218.6" customHeight="1">
       <c r="A45" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B45" s="13">
         <v>4</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E45" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F45" t="s" s="12">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" ht="323" customHeight="1">
@@ -4491,10 +4494,10 @@
       </c>
       <c r="C46" s="4"/>
       <c r="D46" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E46" t="s" s="12">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F46" s="15"/>
     </row>
@@ -4505,51 +4508,51 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s" s="12">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F47" s="15"/>
     </row>
     <row r="48" ht="816" customHeight="1">
       <c r="A48" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B48" s="13">
         <v>3</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48" t="s" s="12">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F48" t="s" s="12">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" ht="170" customHeight="1">
       <c r="A49" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B49" s="13">
         <v>3</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E49" t="s" s="12">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F49" t="s" s="12">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" ht="187" customHeight="1">
@@ -4559,10 +4562,10 @@
       </c>
       <c r="C50" s="4"/>
       <c r="D50" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E50" t="s" s="12">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F50" s="15"/>
     </row>
@@ -4573,71 +4576,71 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E51" t="s" s="12">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F51" s="15"/>
     </row>
     <row r="52" ht="187" customHeight="1">
       <c r="A52" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B52" s="13">
         <v>4</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D52" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E52" t="s" s="12">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F52" t="s" s="12">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" ht="17" customHeight="1">
       <c r="A53" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B53" s="13">
         <v>4</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E53" t="s" s="12">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" ht="187" customHeight="1">
       <c r="A54" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B54" s="13">
         <v>4</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D54" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E54" t="s" s="12">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F54" t="s" s="12">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" ht="187" customHeight="1">
@@ -4647,31 +4650,31 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E55" t="s" s="12">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F55" s="15"/>
     </row>
     <row r="56" ht="187" customHeight="1">
       <c r="A56" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B56" s="13">
         <v>4</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E56" t="s" s="12">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F56" t="s" s="12">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" ht="136" customHeight="1">
@@ -4681,51 +4684,51 @@
       </c>
       <c r="C57" s="4"/>
       <c r="D57" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E57" t="s" s="12">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F57" s="15"/>
     </row>
     <row r="58" ht="136" customHeight="1">
       <c r="A58" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B58" s="13">
         <v>4</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E58" t="s" s="12">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F58" t="s" s="12">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" ht="17" customHeight="1">
       <c r="A59" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B59" s="13">
         <v>4</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E59" t="s" s="12">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" ht="204" customHeight="1">
@@ -4735,10 +4738,10 @@
       </c>
       <c r="C60" s="4"/>
       <c r="D60" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E60" t="s" s="12">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F60" s="15"/>
     </row>
@@ -4749,191 +4752,191 @@
       </c>
       <c r="C61" s="4"/>
       <c r="D61" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E61" t="s" s="12">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F61" s="15"/>
     </row>
     <row r="62" ht="204" customHeight="1">
       <c r="A62" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B62" s="13">
         <v>4</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E62" t="s" s="12">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F62" t="s" s="12">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" ht="170" customHeight="1">
       <c r="A63" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B63" s="13">
         <v>4</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E63" t="s" s="12">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F63" t="s" s="12">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" ht="187" customHeight="1">
       <c r="A64" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B64" s="13">
         <v>4</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D64" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E64" t="s" s="12">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F64" t="s" s="12">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" ht="187" customHeight="1">
       <c r="A65" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B65" s="13">
         <v>4</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D65" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E65" t="s" s="12">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F65" t="s" s="12">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" ht="17" customHeight="1">
       <c r="A66" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B66" s="13">
         <v>4</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D66" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E66" t="s" s="12">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" ht="221" customHeight="1">
       <c r="A67" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B67" s="13">
         <v>4</v>
       </c>
       <c r="C67" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E67" t="s" s="12">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F67" t="s" s="12">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" ht="221" customHeight="1">
       <c r="A68" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B68" s="13">
         <v>4</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D68" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E68" t="s" s="12">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F68" t="s" s="12">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" ht="17" customHeight="1">
       <c r="A69" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B69" s="13">
         <v>4</v>
       </c>
       <c r="C69" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D69" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E69" t="s" s="12">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" ht="289" customHeight="1">
       <c r="A70" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B70" s="13">
         <v>4</v>
       </c>
       <c r="C70" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D70" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E70" t="s" s="12">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F70" t="s" s="12">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" ht="289" customHeight="1">
@@ -4943,31 +4946,31 @@
       </c>
       <c r="C71" s="4"/>
       <c r="D71" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E71" t="s" s="12">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F71" s="15"/>
     </row>
     <row r="72" ht="289" customHeight="1">
       <c r="A72" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B72" s="13">
         <v>4</v>
       </c>
       <c r="C72" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D72" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E72" t="s" s="12">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F72" t="s" s="12">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" ht="187" customHeight="1">
@@ -4977,91 +4980,91 @@
       </c>
       <c r="C73" s="4"/>
       <c r="D73" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E73" t="s" s="12">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F73" s="15"/>
     </row>
     <row r="74" ht="187" customHeight="1">
       <c r="A74" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B74" s="13">
         <v>4</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D74" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E74" t="s" s="12">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F74" t="s" s="12">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" ht="187" customHeight="1">
       <c r="A75" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B75" s="13">
         <v>4</v>
       </c>
       <c r="C75" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D75" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E75" t="s" s="12">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F75" t="s" s="12">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" ht="187" customHeight="1">
       <c r="A76" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B76" s="13">
         <v>4</v>
       </c>
       <c r="C76" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D76" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E76" t="s" s="12">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F76" t="s" s="12">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" ht="17" customHeight="1">
       <c r="A77" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B77" s="13">
         <v>4</v>
       </c>
       <c r="C77" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D77" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E77" t="s" s="12">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" ht="221" customHeight="1">
@@ -5071,10 +5074,10 @@
       </c>
       <c r="C78" s="4"/>
       <c r="D78" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E78" t="s" s="12">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F78" s="15"/>
     </row>
@@ -5085,51 +5088,51 @@
       </c>
       <c r="C79" s="4"/>
       <c r="D79" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E79" t="s" s="12">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F79" s="15"/>
     </row>
     <row r="80" ht="221" customHeight="1">
       <c r="A80" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B80" s="13">
         <v>4</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D80" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E80" t="s" s="12">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F80" t="s" s="12">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" ht="153" customHeight="1">
       <c r="A81" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B81" s="13">
         <v>4</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D81" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E81" t="s" s="12">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F81" t="s" s="12">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" ht="153" customHeight="1">
@@ -5139,31 +5142,31 @@
       </c>
       <c r="C82" s="4"/>
       <c r="D82" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E82" t="s" s="12">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F82" s="15"/>
     </row>
     <row r="83" ht="153" customHeight="1">
       <c r="A83" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B83" s="13">
         <v>4</v>
       </c>
       <c r="C83" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D83" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E83" t="s" s="12">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F83" t="s" s="12">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" ht="153" customHeight="1">
@@ -5173,111 +5176,111 @@
       </c>
       <c r="C84" s="4"/>
       <c r="D84" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E84" t="s" s="12">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F84" s="15"/>
     </row>
     <row r="85" ht="153" customHeight="1">
       <c r="A85" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B85" s="13">
         <v>4</v>
       </c>
       <c r="C85" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D85" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E85" t="s" s="12">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F85" t="s" s="12">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" ht="153" customHeight="1">
       <c r="A86" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B86" s="13">
         <v>4</v>
       </c>
       <c r="C86" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D86" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E86" t="s" s="12">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F86" t="s" s="12">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87" ht="153" customHeight="1">
       <c r="A87" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B87" s="13">
         <v>4</v>
       </c>
       <c r="C87" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D87" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E87" t="s" s="12">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F87" t="s" s="12">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="88" ht="153" customHeight="1">
       <c r="A88" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B88" s="13">
         <v>4</v>
       </c>
       <c r="C88" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D88" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E88" t="s" s="12">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F88" t="s" s="12">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" ht="153" customHeight="1">
       <c r="A89" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B89" s="13">
         <v>4</v>
       </c>
       <c r="C89" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D89" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E89" t="s" s="12">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F89" t="s" s="12">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" ht="153" customHeight="1">
@@ -5287,71 +5290,71 @@
       </c>
       <c r="C90" s="4"/>
       <c r="D90" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E90" t="s" s="12">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F90" s="15"/>
     </row>
     <row r="91" ht="153" customHeight="1">
       <c r="A91" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B91" s="13">
         <v>3</v>
       </c>
       <c r="C91" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E91" t="s" s="12">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F91" t="s" s="12">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="92" ht="153" customHeight="1">
       <c r="A92" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B92" s="13">
         <v>3</v>
       </c>
       <c r="C92" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D92" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E92" t="s" s="12">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F92" t="s" s="12">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="93" ht="153" customHeight="1">
       <c r="A93" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B93" s="13">
         <v>3</v>
       </c>
       <c r="C93" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D93" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E93" t="s" s="12">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F93" t="s" s="12">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" ht="153" customHeight="1">
@@ -5361,31 +5364,31 @@
       </c>
       <c r="C94" s="4"/>
       <c r="D94" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E94" t="s" s="12">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F94" s="15"/>
     </row>
     <row r="95" ht="153" customHeight="1">
       <c r="A95" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B95" s="13">
         <v>3</v>
       </c>
       <c r="C95" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D95" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E95" t="s" s="12">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F95" t="s" s="12">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" ht="153" customHeight="1">
@@ -5395,71 +5398,71 @@
       </c>
       <c r="C96" s="4"/>
       <c r="D96" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E96" t="s" s="12">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F96" s="15"/>
     </row>
     <row r="97" ht="153" customHeight="1">
       <c r="A97" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B97" s="13">
         <v>2</v>
       </c>
       <c r="C97" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D97" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E97" t="s" s="12">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F97" t="s" s="12">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" ht="153" customHeight="1">
       <c r="A98" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B98" s="13">
         <v>2</v>
       </c>
       <c r="C98" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D98" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E98" t="s" s="12">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F98" t="s" s="12">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="99" ht="153" customHeight="1">
       <c r="A99" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B99" s="13">
         <v>2</v>
       </c>
       <c r="C99" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D99" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E99" t="s" s="12">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F99" t="s" s="12">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" ht="153" customHeight="1">
@@ -5469,51 +5472,51 @@
       </c>
       <c r="C100" s="4"/>
       <c r="D100" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E100" t="s" s="12">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F100" s="15"/>
     </row>
     <row r="101" ht="153" customHeight="1">
       <c r="A101" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B101" s="13">
         <v>3</v>
       </c>
       <c r="C101" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D101" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E101" t="s" s="12">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F101" t="s" s="12">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="102" ht="153" customHeight="1">
       <c r="A102" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B102" s="13">
         <v>3</v>
       </c>
       <c r="C102" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D102" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E102" t="s" s="12">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F102" t="s" s="12">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="103" ht="153" customHeight="1">
@@ -5523,10 +5526,10 @@
       </c>
       <c r="C103" s="4"/>
       <c r="D103" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E103" t="s" s="12">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F103" s="15"/>
     </row>
@@ -5537,51 +5540,51 @@
       </c>
       <c r="C104" s="4"/>
       <c r="D104" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E104" t="s" s="12">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F104" s="15"/>
     </row>
     <row r="105" ht="153" customHeight="1">
       <c r="A105" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B105" s="13">
         <v>4</v>
       </c>
       <c r="C105" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D105" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E105" t="s" s="12">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F105" t="s" s="12">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" ht="153" customHeight="1">
       <c r="A106" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B106" s="13">
         <v>4</v>
       </c>
       <c r="C106" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D106" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E106" t="s" s="12">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F106" t="s" s="12">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="107" ht="153" customHeight="1">
@@ -5591,51 +5594,51 @@
       </c>
       <c r="C107" s="4"/>
       <c r="D107" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E107" t="s" s="12">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F107" s="15"/>
     </row>
     <row r="108" ht="153" customHeight="1">
       <c r="A108" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B108" s="13">
         <v>4</v>
       </c>
       <c r="C108" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D108" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E108" t="s" s="12">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F108" t="s" s="12">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="109" ht="153" customHeight="1">
       <c r="A109" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B109" s="13">
         <v>4</v>
       </c>
       <c r="C109" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D109" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E109" t="s" s="12">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F109" t="s" s="12">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" ht="153" customHeight="1">
@@ -5645,71 +5648,71 @@
       </c>
       <c r="C110" s="4"/>
       <c r="D110" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E110" t="s" s="12">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F110" s="15"/>
     </row>
     <row r="111" ht="153" customHeight="1">
       <c r="A111" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B111" s="13">
         <v>4</v>
       </c>
       <c r="C111" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D111" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E111" t="s" s="12">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F111" t="s" s="12">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="112" ht="153" customHeight="1">
       <c r="A112" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B112" s="13">
         <v>4</v>
       </c>
       <c r="C112" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D112" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E112" t="s" s="12">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F112" t="s" s="12">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" ht="153" customHeight="1">
       <c r="A113" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B113" s="13">
         <v>4</v>
       </c>
       <c r="C113" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D113" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E113" t="s" s="12">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F113" t="s" s="12">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="114" ht="153" customHeight="1">
@@ -5719,51 +5722,51 @@
       </c>
       <c r="C114" s="4"/>
       <c r="D114" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E114" t="s" s="12">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F114" s="15"/>
     </row>
     <row r="115" ht="153" customHeight="1">
       <c r="A115" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B115" s="13">
         <v>4</v>
       </c>
       <c r="C115" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D115" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E115" t="s" s="12">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F115" t="s" s="12">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="116" ht="153" customHeight="1">
       <c r="A116" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B116" s="13">
         <v>4</v>
       </c>
       <c r="C116" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D116" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E116" t="s" s="12">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F116" t="s" s="12">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="117" ht="153" customHeight="1">
@@ -5773,51 +5776,51 @@
       </c>
       <c r="C117" s="4"/>
       <c r="D117" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E117" t="s" s="12">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F117" s="15"/>
     </row>
     <row r="118" ht="153" customHeight="1">
       <c r="A118" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B118" s="13">
         <v>4</v>
       </c>
       <c r="C118" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D118" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E118" t="s" s="12">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F118" t="s" s="12">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="119" ht="153" customHeight="1">
       <c r="A119" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B119" s="13">
         <v>4</v>
       </c>
       <c r="C119" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D119" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E119" t="s" s="12">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F119" t="s" s="12">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" ht="153" customHeight="1">
@@ -5827,71 +5830,71 @@
       </c>
       <c r="C120" s="4"/>
       <c r="D120" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E120" t="s" s="12">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F120" s="15"/>
     </row>
     <row r="121" ht="153" customHeight="1">
       <c r="A121" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B121" s="13">
         <v>3</v>
       </c>
       <c r="C121" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D121" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E121" t="s" s="12">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F121" t="s" s="12">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" ht="153" customHeight="1">
       <c r="A122" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B122" s="13">
         <v>3</v>
       </c>
       <c r="C122" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D122" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E122" t="s" s="12">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F122" t="s" s="12">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="123" ht="153" customHeight="1">
       <c r="A123" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B123" s="13">
         <v>3</v>
       </c>
       <c r="C123" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D123" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E123" t="s" s="12">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F123" t="s" s="12">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="124" ht="153" customHeight="1">
@@ -8042,23 +8045,23 @@
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -8066,10 +8069,10 @@
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -8077,10 +8080,10 @@
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -8088,10 +8091,10 @@
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>

</xml_diff>